<commit_message>
power point, cambios menores para ajustar diseño
</commit_message>
<xml_diff>
--- a/por hacer.xlsx
+++ b/por hacer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Visual\proyecto\proyecto_skills_2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF36A5C-68AB-426A-95B7-AD81603172D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81CA9033-F5BE-4D53-87D5-C7C4EB251F83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Landing page</t>
   </si>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>Un logotipo de Spain Skill</t>
-  </si>
-  <si>
-    <t>Una imagen de promoción de alguno de los juegos que podrá ir cambiando con el tiempo (provistas en la carpeta de datos).</t>
   </si>
   <si>
     <t xml:space="preserve">Una animación interactiva creada con un personaje de estética “retro” (se incluyen imágenes del mismo) que recoge varios objetos por la pantalla. </t>
@@ -126,18 +123,12 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -158,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -167,9 +158,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -512,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AH171"/>
+  <dimension ref="A1:AH170"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,16 +549,16 @@
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -599,16 +587,16 @@
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="3"/>
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
@@ -637,16 +625,16 @@
     </row>
     <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="3"/>
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -675,16 +663,16 @@
     </row>
     <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
+      <c r="B5" s="3"/>
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -714,15 +702,15 @@
     <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3"/>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -751,16 +739,16 @@
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -789,16 +777,16 @@
     </row>
     <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3"/>
+      <c r="C8" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -827,16 +815,16 @@
     </row>
     <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -865,9 +853,9 @@
     </row>
     <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="4"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="5" t="s">
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="5"/>
@@ -903,16 +891,16 @@
     </row>
     <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="6" t="s">
+      <c r="B11" s="3"/>
+      <c r="C11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
@@ -941,16 +929,16 @@
     </row>
     <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="5" t="s">
-        <v>27</v>
+      <c r="B12" s="4" t="s">
+        <v>8</v>
       </c>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
@@ -979,16 +967,16 @@
     </row>
     <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="3"/>
+      <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1"/>
@@ -1017,17 +1005,17 @@
     </row>
     <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
-        <v>10</v>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4" t="s">
+        <v>17</v>
       </c>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="1"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="2"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
@@ -1055,17 +1043,17 @@
     </row>
     <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
-        <v>18</v>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="2"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1"/>
       <c r="M15" s="1"/>
@@ -1093,16 +1081,16 @@
     </row>
     <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
+      <c r="B16" s="3"/>
+      <c r="C16" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
@@ -1131,16 +1119,16 @@
     </row>
     <row r="17" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
-        <v>12</v>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4" t="s">
+        <v>13</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
@@ -1169,16 +1157,16 @@
     </row>
     <row r="18" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
-        <v>14</v>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4" t="s">
+        <v>12</v>
       </c>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
@@ -1208,15 +1196,15 @@
     <row r="19" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3"/>
-      <c r="C19" s="5" t="s">
-        <v>13</v>
+      <c r="C19" s="4" t="s">
+        <v>14</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
@@ -1246,15 +1234,15 @@
     <row r="20" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3"/>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
       <c r="L20" s="1"/>
@@ -1284,15 +1272,15 @@
     <row r="21" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3"/>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
@@ -1321,16 +1309,16 @@
     </row>
     <row r="22" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
-      <c r="B22" s="4"/>
-      <c r="C22" s="5" t="s">
-        <v>17</v>
+      <c r="B22" s="4" t="s">
+        <v>18</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
@@ -1359,16 +1347,16 @@
     </row>
     <row r="23" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="3"/>
+      <c r="C23" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
@@ -1397,16 +1385,16 @@
     </row>
     <row r="24" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
-      <c r="B24" s="4"/>
-      <c r="C24" s="5" t="s">
+      <c r="B24" s="3"/>
+      <c r="C24" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="5"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
@@ -1435,16 +1423,16 @@
     </row>
     <row r="25" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="5" t="s">
-        <v>21</v>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4" t="s">
+        <v>24</v>
       </c>
-      <c r="D25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="5"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
@@ -1473,16 +1461,16 @@
     </row>
     <row r="26" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="5" t="s">
-        <v>25</v>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4" t="s">
+        <v>21</v>
       </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="5"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
@@ -1512,15 +1500,15 @@
     <row r="27" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="5"/>
-      <c r="G27" s="5"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="5"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
@@ -1550,15 +1538,15 @@
     <row r="28" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
@@ -1587,16 +1575,14 @@
     </row>
     <row r="29" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
@@ -1626,13 +1612,13 @@
     <row r="30" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
@@ -1662,13 +1648,13 @@
     <row r="31" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
@@ -1698,13 +1684,13 @@
     <row r="32" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
@@ -1734,13 +1720,13 @@
     <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
@@ -1770,13 +1756,13 @@
     <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
@@ -1806,13 +1792,13 @@
     <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -1842,13 +1828,13 @@
     <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
       <c r="L36" s="1"/>
@@ -1878,13 +1864,13 @@
     <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
@@ -1914,13 +1900,13 @@
     <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
       <c r="L38" s="1"/>
@@ -1950,13 +1936,13 @@
     <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
@@ -1986,13 +1972,13 @@
     <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
-      <c r="I40" s="5"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
       <c r="L40" s="1"/>
@@ -2022,13 +2008,13 @@
     <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="5"/>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
-      <c r="I41" s="5"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
@@ -2058,13 +2044,13 @@
     <row r="42" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
-      <c r="E42" s="5"/>
-      <c r="F42" s="5"/>
-      <c r="G42" s="5"/>
-      <c r="H42" s="5"/>
-      <c r="I42" s="5"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
@@ -2094,13 +2080,13 @@
     <row r="43" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
-      <c r="I43" s="5"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
       <c r="L43" s="1"/>
@@ -2130,13 +2116,13 @@
     <row r="44" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
-      <c r="I44" s="5"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
@@ -2166,13 +2152,13 @@
     <row r="45" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
-      <c r="I45" s="5"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
@@ -2202,13 +2188,13 @@
     <row r="46" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
-      <c r="I46" s="5"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
@@ -2238,13 +2224,13 @@
     <row r="47" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
-      <c r="I47" s="5"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
@@ -2274,13 +2260,13 @@
     <row r="48" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
@@ -2310,13 +2296,13 @@
     <row r="49" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
-      <c r="I49" s="5"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
+      <c r="E49" s="4"/>
+      <c r="F49" s="4"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
       <c r="L49" s="1"/>
@@ -2346,13 +2332,13 @@
     <row r="50" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
       <c r="L50" s="1"/>
@@ -2382,13 +2368,13 @@
     <row r="51" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
       <c r="L51" s="1"/>
@@ -2418,13 +2404,13 @@
     <row r="52" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5"/>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5"/>
-      <c r="I52" s="5"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
+      <c r="E52" s="4"/>
+      <c r="F52" s="4"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
       <c r="L52" s="1"/>
@@ -2454,13 +2440,13 @@
     <row r="53" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
-      <c r="E53" s="5"/>
-      <c r="F53" s="5"/>
-      <c r="G53" s="5"/>
-      <c r="H53" s="5"/>
-      <c r="I53" s="5"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
+      <c r="E53" s="4"/>
+      <c r="F53" s="4"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
@@ -2490,13 +2476,13 @@
     <row r="54" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="5"/>
-      <c r="F54" s="5"/>
-      <c r="G54" s="5"/>
-      <c r="H54" s="5"/>
-      <c r="I54" s="5"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
+      <c r="E54" s="4"/>
+      <c r="F54" s="4"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
@@ -2526,13 +2512,13 @@
     <row r="55" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="5"/>
-      <c r="F55" s="5"/>
-      <c r="G55" s="5"/>
-      <c r="H55" s="5"/>
-      <c r="I55" s="5"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
@@ -2562,13 +2548,13 @@
     <row r="56" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
-      <c r="C56" s="5"/>
-      <c r="D56" s="5"/>
-      <c r="E56" s="5"/>
-      <c r="F56" s="5"/>
-      <c r="G56" s="5"/>
-      <c r="H56" s="5"/>
-      <c r="I56" s="5"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="4"/>
+      <c r="F56" s="4"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
@@ -2598,13 +2584,13 @@
     <row r="57" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="5"/>
-      <c r="F57" s="5"/>
-      <c r="G57" s="5"/>
-      <c r="H57" s="5"/>
-      <c r="I57" s="5"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
+      <c r="E57" s="4"/>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
       <c r="L57" s="1"/>
@@ -2634,13 +2620,13 @@
     <row r="58" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
-      <c r="E58" s="5"/>
-      <c r="F58" s="5"/>
-      <c r="G58" s="5"/>
-      <c r="H58" s="5"/>
-      <c r="I58" s="5"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
+      <c r="E58" s="4"/>
+      <c r="F58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
@@ -2670,13 +2656,13 @@
     <row r="59" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="5"/>
-      <c r="F59" s="5"/>
-      <c r="G59" s="5"/>
-      <c r="H59" s="5"/>
-      <c r="I59" s="5"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="4"/>
+      <c r="F59" s="4"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
@@ -2706,13 +2692,13 @@
     <row r="60" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
+      <c r="E60" s="4"/>
+      <c r="F60" s="4"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
@@ -2742,13 +2728,13 @@
     <row r="61" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
-      <c r="E61" s="5"/>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
+      <c r="E61" s="4"/>
+      <c r="F61" s="4"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
       <c r="L61" s="1"/>
@@ -2778,13 +2764,13 @@
     <row r="62" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="5"/>
-      <c r="F62" s="5"/>
-      <c r="G62" s="5"/>
-      <c r="H62" s="5"/>
-      <c r="I62" s="5"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
@@ -2814,13 +2800,13 @@
     <row r="63" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4"/>
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
@@ -2850,13 +2836,13 @@
     <row r="64" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
-      <c r="C64" s="5"/>
-      <c r="D64" s="5"/>
-      <c r="E64" s="5"/>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
+      <c r="E64" s="4"/>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4"/>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
       <c r="L64" s="1"/>
@@ -2886,13 +2872,13 @@
     <row r="65" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="5"/>
-      <c r="F65" s="5"/>
-      <c r="G65" s="5"/>
-      <c r="H65" s="5"/>
-      <c r="I65" s="5"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -2922,13 +2908,13 @@
     <row r="66" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
-      <c r="E66" s="5"/>
-      <c r="F66" s="5"/>
-      <c r="G66" s="5"/>
-      <c r="H66" s="5"/>
-      <c r="I66" s="5"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
+      <c r="E66" s="4"/>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4"/>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
@@ -2958,13 +2944,13 @@
     <row r="67" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="5"/>
-      <c r="F67" s="5"/>
-      <c r="G67" s="5"/>
-      <c r="H67" s="5"/>
-      <c r="I67" s="5"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4"/>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4"/>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
       <c r="L67" s="1"/>
@@ -2994,13 +2980,13 @@
     <row r="68" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="5"/>
-      <c r="F68" s="5"/>
-      <c r="G68" s="5"/>
-      <c r="H68" s="5"/>
-      <c r="I68" s="5"/>
+      <c r="C68" s="4"/>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
+      <c r="F68" s="4"/>
+      <c r="G68" s="4"/>
+      <c r="H68" s="4"/>
+      <c r="I68" s="4"/>
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
       <c r="L68" s="1"/>
@@ -3030,13 +3016,13 @@
     <row r="69" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
-      <c r="E69" s="5"/>
-      <c r="F69" s="5"/>
-      <c r="G69" s="5"/>
-      <c r="H69" s="5"/>
-      <c r="I69" s="5"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="4"/>
+      <c r="F69" s="4"/>
+      <c r="G69" s="4"/>
+      <c r="H69" s="4"/>
+      <c r="I69" s="4"/>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
@@ -3066,13 +3052,13 @@
     <row r="70" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="5"/>
-      <c r="F70" s="5"/>
-      <c r="G70" s="5"/>
-      <c r="H70" s="5"/>
-      <c r="I70" s="5"/>
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
+      <c r="G70" s="4"/>
+      <c r="H70" s="4"/>
+      <c r="I70" s="4"/>
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
@@ -3102,13 +3088,13 @@
     <row r="71" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="5"/>
-      <c r="F71" s="5"/>
-      <c r="G71" s="5"/>
-      <c r="H71" s="5"/>
-      <c r="I71" s="5"/>
+      <c r="C71" s="4"/>
+      <c r="D71" s="4"/>
+      <c r="E71" s="4"/>
+      <c r="F71" s="4"/>
+      <c r="G71" s="4"/>
+      <c r="H71" s="4"/>
+      <c r="I71" s="4"/>
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
@@ -3138,13 +3124,13 @@
     <row r="72" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
-      <c r="C72" s="5"/>
-      <c r="D72" s="5"/>
-      <c r="E72" s="5"/>
-      <c r="F72" s="5"/>
-      <c r="G72" s="5"/>
-      <c r="H72" s="5"/>
-      <c r="I72" s="5"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="4"/>
+      <c r="F72" s="4"/>
+      <c r="G72" s="4"/>
+      <c r="H72" s="4"/>
+      <c r="I72" s="4"/>
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
       <c r="L72" s="1"/>
@@ -3174,13 +3160,13 @@
     <row r="73" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="5"/>
-      <c r="F73" s="5"/>
-      <c r="G73" s="5"/>
-      <c r="H73" s="5"/>
-      <c r="I73" s="5"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+      <c r="E73" s="4"/>
+      <c r="F73" s="4"/>
+      <c r="G73" s="4"/>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4"/>
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
@@ -3210,13 +3196,13 @@
     <row r="74" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
-      <c r="E74" s="5"/>
-      <c r="F74" s="5"/>
-      <c r="G74" s="5"/>
-      <c r="H74" s="5"/>
-      <c r="I74" s="5"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+      <c r="E74" s="4"/>
+      <c r="F74" s="4"/>
+      <c r="G74" s="4"/>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
       <c r="L74" s="1"/>
@@ -3246,13 +3232,13 @@
     <row r="75" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
-      <c r="E75" s="5"/>
-      <c r="F75" s="5"/>
-      <c r="G75" s="5"/>
-      <c r="H75" s="5"/>
-      <c r="I75" s="5"/>
+      <c r="C75" s="4"/>
+      <c r="D75" s="4"/>
+      <c r="E75" s="4"/>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
       <c r="L75" s="1"/>
@@ -3282,13 +3268,13 @@
     <row r="76" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
-      <c r="E76" s="5"/>
-      <c r="F76" s="5"/>
-      <c r="G76" s="5"/>
-      <c r="H76" s="5"/>
-      <c r="I76" s="5"/>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
@@ -3318,13 +3304,13 @@
     <row r="77" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
-      <c r="E77" s="5"/>
-      <c r="F77" s="5"/>
-      <c r="G77" s="5"/>
-      <c r="H77" s="5"/>
-      <c r="I77" s="5"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
+      <c r="G77" s="4"/>
+      <c r="H77" s="4"/>
+      <c r="I77" s="4"/>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
       <c r="L77" s="1"/>
@@ -3354,13 +3340,13 @@
     <row r="78" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
-      <c r="E78" s="5"/>
-      <c r="F78" s="5"/>
-      <c r="G78" s="5"/>
-      <c r="H78" s="5"/>
-      <c r="I78" s="5"/>
+      <c r="C78" s="4"/>
+      <c r="D78" s="4"/>
+      <c r="E78" s="4"/>
+      <c r="F78" s="4"/>
+      <c r="G78" s="4"/>
+      <c r="H78" s="4"/>
+      <c r="I78" s="4"/>
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
@@ -3390,13 +3376,13 @@
     <row r="79" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5"/>
-      <c r="E79" s="5"/>
-      <c r="F79" s="5"/>
-      <c r="G79" s="5"/>
-      <c r="H79" s="5"/>
-      <c r="I79" s="5"/>
+      <c r="C79" s="4"/>
+      <c r="D79" s="4"/>
+      <c r="E79" s="4"/>
+      <c r="F79" s="4"/>
+      <c r="G79" s="4"/>
+      <c r="H79" s="4"/>
+      <c r="I79" s="4"/>
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
       <c r="L79" s="1"/>
@@ -3426,13 +3412,13 @@
     <row r="80" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
-      <c r="C80" s="5"/>
-      <c r="D80" s="5"/>
-      <c r="E80" s="5"/>
-      <c r="F80" s="5"/>
-      <c r="G80" s="5"/>
-      <c r="H80" s="5"/>
-      <c r="I80" s="5"/>
+      <c r="C80" s="4"/>
+      <c r="D80" s="4"/>
+      <c r="E80" s="4"/>
+      <c r="F80" s="4"/>
+      <c r="G80" s="4"/>
+      <c r="H80" s="4"/>
+      <c r="I80" s="4"/>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
       <c r="L80" s="1"/>
@@ -3462,13 +3448,13 @@
     <row r="81" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
-      <c r="E81" s="5"/>
-      <c r="F81" s="5"/>
-      <c r="G81" s="5"/>
-      <c r="H81" s="5"/>
-      <c r="I81" s="5"/>
+      <c r="C81" s="4"/>
+      <c r="D81" s="4"/>
+      <c r="E81" s="4"/>
+      <c r="F81" s="4"/>
+      <c r="G81" s="4"/>
+      <c r="H81" s="4"/>
+      <c r="I81" s="4"/>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
@@ -3498,13 +3484,13 @@
     <row r="82" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="5"/>
-      <c r="G82" s="5"/>
-      <c r="H82" s="5"/>
-      <c r="I82" s="5"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="H82" s="1"/>
+      <c r="I82" s="1"/>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
       <c r="L82" s="1"/>
@@ -6664,8 +6650,6 @@
       <c r="AH169" s="1"/>
     </row>
     <row r="170" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
-      <c r="B170" s="1"/>
       <c r="C170" s="1"/>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
@@ -6673,63 +6657,29 @@
       <c r="G170" s="1"/>
       <c r="H170" s="1"/>
       <c r="I170" s="1"/>
-      <c r="J170" s="1"/>
-      <c r="K170" s="1"/>
-      <c r="L170" s="1"/>
-      <c r="M170" s="1"/>
-      <c r="N170" s="1"/>
-      <c r="O170" s="1"/>
-      <c r="P170" s="1"/>
-      <c r="Q170" s="1"/>
-      <c r="R170" s="1"/>
-      <c r="S170" s="1"/>
-      <c r="T170" s="1"/>
-      <c r="U170" s="1"/>
-      <c r="V170" s="1"/>
-      <c r="W170" s="1"/>
-      <c r="X170" s="1"/>
-      <c r="Y170" s="1"/>
-      <c r="Z170" s="1"/>
-      <c r="AA170" s="1"/>
-      <c r="AB170" s="1"/>
-      <c r="AC170" s="1"/>
-      <c r="AD170" s="1"/>
-      <c r="AE170" s="1"/>
-      <c r="AF170" s="1"/>
-      <c r="AG170" s="1"/>
-      <c r="AH170" s="1"/>
-    </row>
-    <row r="171" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="C171" s="1"/>
-      <c r="D171" s="1"/>
-      <c r="E171" s="1"/>
-      <c r="F171" s="1"/>
-      <c r="G171" s="1"/>
-      <c r="H171" s="1"/>
-      <c r="I171" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="81">
+  <mergeCells count="80">
+    <mergeCell ref="C20:I20"/>
     <mergeCell ref="C21:I21"/>
-    <mergeCell ref="C22:I22"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="C14:I14"/>
-    <mergeCell ref="C16:I16"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="C13:I13"/>
+    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C17:I17"/>
     <mergeCell ref="C18:I18"/>
     <mergeCell ref="C19:I19"/>
-    <mergeCell ref="C20:I20"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="C15:I15"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C14:I14"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="C5:I5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="B8:I8"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="C8:I8"/>
     <mergeCell ref="C9:I9"/>
     <mergeCell ref="C10:I10"/>
     <mergeCell ref="C11:I11"/>
-    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="C23:I23"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="C25:I25"/>
     <mergeCell ref="C26:I26"/>
@@ -6758,39 +6708,38 @@
     <mergeCell ref="C49:I49"/>
     <mergeCell ref="C50:I50"/>
     <mergeCell ref="C51:I51"/>
-    <mergeCell ref="C52:I52"/>
+    <mergeCell ref="C58:I58"/>
     <mergeCell ref="C59:I59"/>
     <mergeCell ref="C60:I60"/>
     <mergeCell ref="C61:I61"/>
-    <mergeCell ref="C62:I62"/>
+    <mergeCell ref="C52:I52"/>
     <mergeCell ref="C53:I53"/>
     <mergeCell ref="C54:I54"/>
     <mergeCell ref="C55:I55"/>
     <mergeCell ref="C56:I56"/>
-    <mergeCell ref="C57:I57"/>
+    <mergeCell ref="C80:I80"/>
     <mergeCell ref="C81:I81"/>
-    <mergeCell ref="C82:I82"/>
+    <mergeCell ref="C72:I72"/>
     <mergeCell ref="C73:I73"/>
     <mergeCell ref="C74:I74"/>
     <mergeCell ref="C75:I75"/>
     <mergeCell ref="C76:I76"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="C16:I16"/>
     <mergeCell ref="C77:I77"/>
-    <mergeCell ref="B23:I23"/>
-    <mergeCell ref="C17:I17"/>
     <mergeCell ref="C78:I78"/>
     <mergeCell ref="C79:I79"/>
-    <mergeCell ref="C80:I80"/>
+    <mergeCell ref="C67:I67"/>
     <mergeCell ref="C68:I68"/>
     <mergeCell ref="C69:I69"/>
     <mergeCell ref="C70:I70"/>
     <mergeCell ref="C71:I71"/>
-    <mergeCell ref="C72:I72"/>
+    <mergeCell ref="C62:I62"/>
     <mergeCell ref="C63:I63"/>
     <mergeCell ref="C64:I64"/>
     <mergeCell ref="C65:I65"/>
     <mergeCell ref="C66:I66"/>
-    <mergeCell ref="C67:I67"/>
-    <mergeCell ref="C58:I58"/>
+    <mergeCell ref="C57:I57"/>
   </mergeCells>
   <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75" bottom="0.75" header="0.30000000000000004" footer="0.30000000000000004"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>